<commit_message>
commit last couple of months
</commit_message>
<xml_diff>
--- a/stage/Logblad_Stage.xlsx
+++ b/stage/Logblad_Stage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbelm\Documenten\Graduaat-Programmeren\stage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C212C7E-9030-4512-A6F8-7825D4348128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCFD3C9-DA9F-4DEC-BF49-3223FD328D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{17B13AA9-2AFD-4646-A20A-7BB5FF3EC105}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{17B13AA9-2AFD-4646-A20A-7BB5FF3EC105}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="175">
   <si>
     <t>Logblad Stage</t>
   </si>
@@ -547,10 +547,16 @@
 page wanneer je meer bestanden hebt dan dat je scherm groot is</t>
   </si>
   <si>
-    <t>Vandaag heb ik verder gedaan met het fixing van bugs. ik volgende 4 bugs gefixt
+    <t>graduaatsproef</t>
+  </si>
+  <si>
+    <t>Vandaag heb ik heel de dag mogen werken aan mijn graduaatsproef</t>
+  </si>
+  <si>
+    <t>Vandaag heb ik verder gedaan met het fixing van bugs. ik heb de volgende 4 bugs gefixt
 Er stond bij ondersteunende talen chinees tussen waardoor sommige gebruikers soms hun
 bestanden in het chinees zagen, dat heb ik aangepast door het chinees te verwijderen
-van ondersteunende talen. Een ander probleem was dat er geen validation was bi het invullen
+van ondersteunende talen. Een ander probleem was dat er geen validation was bij het invullen
 van enkele velden. Zo kon men alles invullen bij hun naam en email zonder dat deze
 gecontroleerd werd. Dit heb ik aangepast en ook ervoor gezorgd dat je je gsm nummer kan
 aanpassen. Een ander klein probleem was dat de error-message van andere validatie velden
@@ -558,6 +564,184 @@
 probleem van de dag was dat men geen sharecodes kon maken als er geen bestonden. Deze
 probleem kwam omdat je eerst zocht of een sharecode al bestond maar als er geen bestonden
 dan werd er een fout verstuurd ipv de pop-up om één aan te maken</t>
+  </si>
+  <si>
+    <t>Vandaag heb ik verder gedaan met het fixing van enkele bugs. De bug die vandaag
+het langste duurde om op te lossen was eentje waarbij er geen validatie was
+bij het invullen van het adres bij het maken van een nieuw project.
+Dit heb ik opgelost om te controleren of een adres werd aangevuld en die
+correct was. Als die niet correct is krijg je dan een zinnetje met de 
+uitleg waarom het niet correct is.</t>
+  </si>
+  <si>
+    <t>Feature added</t>
+  </si>
+  <si>
+    <t>Vandaag was mijn bezigheid om een feature toe te voegen. Zo heb ik ervoor gezorgd
+dat je nu je profiel, portaal en coverfoto kan verwijderen wat vroeger niet kon.
+Deze feature bracht enkele problemen met zich mee want om iets te verwijderen
+werd dezelfde functie gebruikt, maar de placeholder voor profiel- en portaalfoto
+zijn anders dan die voor de coverfoto, zo moest ik dus een onderscheid maken
+tussen die twee en dat zo meegeven naar de backend zo dat de backend mij de correcte
+placeholder terug stuurde</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vandaag heb ik 3 bugs gefixt, de eerste was een bug dat ervoor
+zorgde dat wanneer je je mail wou verifiëren je naar een blank page
+werd gestuurd. De fout hier zat dat er nog gebruik werd gemaakt van 
+het oude navigatie systeem. Een tweede fout was dat de gebruikers
+op het opslaan knop konden drukken wanneer niet alle verplichte velden
+ingevuld waren, daardoor kwam het programma vast te zitten. Dit heb ik
+opgelost met de button te disabelen tot dat alle verplichte velden ingevuld
+zijn. Als laatste heb ik ook ervoor gezorgd dat de linked icoontje op de foto's
+staat wanneer die gebruikt worden bij een unit. </t>
+  </si>
+  <si>
+    <t>extra seo pages toevoegen</t>
+  </si>
+  <si>
+    <t>Zowel gisteren als vandaag was mijn taak om alle seo pages van
+verschillende steden en provincie toe te voegen. Dit hield in
+om 10 pages te maken voor steden in de provincie Antwerpen.
+Twee provincepages voor de provincies Vlaams-Brabant en Limburg.
+En voor die twee provincies elk nog eens 5 steden.</t>
+  </si>
+  <si>
+    <t>24/04/2025
+&amp;
+25/04/2025</t>
+  </si>
+  <si>
+    <t>Vandaag heb ik volgende twee bugs gefixt. Vroeger kon je alleen de prijs
+aanpassen van een unit in het engelse tablad. Ik heb het nu aangepast dat
+je nu de prijs in elke taal kan aanpassen. Volgende bug dat ik heb gefixt was
+eentje die al sinds mijn tweede stageweek in blocked stond. Het probleem was
+dat de eerste sort-by optie altijd in het nederlands stond (onze default language).
+Dit heb ik vandaag na meerdere  keren te proberen eindelijk kunnen oplossen. Het probleem
+kwam voor omdat de eerste sort-by optie werd geinitialiseerd vooraleer dat de waarde van
+de localizer (waar de gekozen taal door de gebruiker word opgeslagen) werd gelezen en
+daardoor de default waarde (nederlands) gebruikt word</t>
+  </si>
+  <si>
+    <t>features toegevoegd</t>
+  </si>
+  <si>
+    <t>Vandaag mocht ik 2 features toevoegen. Een eerste feature was ervoor zorgen
+dat de volledige datum van de creatie van een leed word getoond. Hiervoor
+werd enkel de dag en maand getoond maar men wou ook het jaar zien. Dit
+heb ik met behulp van een helperfunctie kunnen toevoegen aan de datum en zo
+ervoor gezorgd dat je nu het volledige datum ziet. Het tweede feature dat
+ik heb toegevoegd zijn de in- en uitzoom buttons zichtbaarder op de pdf reader
+gezet. Eerst moest men op een knop drukken om de navigatiebar zichtbaar te maken
+en daarin vond je de knoppen. Veel gebruikers vonden dat te ingewikkeld of vonden
+het gewoonweg niet, dus ik heb de knopen rechts onder de pagina gezet zodat men ze
+direct kan vinden en gebruiken</t>
+  </si>
+  <si>
+    <t>feature toevoegen</t>
+  </si>
+  <si>
+    <t>Vandaag heb ik gewerkt aan een nieuwe feature waarbij een klant, nadat hij een polygon heeft aangemaakt
+en er een foto aan heeft gekoppeld, via een klik op de polygon automatisch wordt doorverwezen naar de gelinkte foto.
+Deze functionaliteit was technisch uitdagend, omdat er aanpassingen nodig waren in meerdere componenten om alles
+correct met elkaar te laten samenwerken.</t>
+  </si>
+  <si>
+    <t>feature afgewerkt + unittesten</t>
+  </si>
+  <si>
+    <t>Vandaag heb ik de feature van gisteren afgewerkt en voorzien van enkele commentaren ter verduidelijking.
+Daarnaast bestond mijn opdracht erin om de bestaande unittests te bekijken en te begrijpen,
+met als doel om nadien zelf unittests te schrijven voor verschillende pagina’s.
+De eerste unittest die ik vandaag heb geschreven, test een eigen ontwikkelde feature die toelaat
+om de profiel-, portaal- en omslagafbeelding van een gebruiker te verwijderen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verdiepen in Vitest en beginnen unittesten </t>
+  </si>
+  <si>
+    <t>Vandaag kreeg ik de opdracht om me te verdiepen in Vitest, een nieuw en verbeterd testplatform in C#
+dat beter is dan de vorige versie die we gebruikten. Ik heb de hele voormiddag besteed aan het verkennen van de documentatie
+en het begrijpen van de basisprincipes. In de namiddag ben ik zelf begonnen met het schrijven van tests vanaf nul.
+In het begin was het erg lastig en kreeg ik 66 fouten, maar met behulp van GitHub, Stack Overflow en andere online bronnen
+kon ik de problemen oplossen. Tegen het einde van de dag slaagde ik erin om 3 tests zonder fouten te laten draaien.</t>
+  </si>
+  <si>
+    <t>Testen afgewerkt + marketplaceusers flow begonnen</t>
+  </si>
+  <si>
+    <t>Vandaag heb ik de eerste twee uur besteed aan het verbeteren van de test van vorige week die fout liep,
+en heb ik ook nog twee nieuwe testen geschreven. Daarna kreeg ik een grotere opdracht waar ik de komende dagen aan mag werken.
+De bedoeling is om een volledige flow op te zetten — van het scherm dat de gebruiker ziet tot aan de backend — 
+om marketplacegebruikers te kunnen beheren. Het uiteindelijke doel is om tegen het einde van de week 
+eautomatiseerde e-mails te versturen naar alle gebruikers die nog geen account hebben, zodat zij er één kunnen aanmaken.
+Het is een uitdagende taak, vooral omdat het de eerste keer is dat ik zo nauw in contact kom met de backend
+en zelf een API-call moet schrijven, maar ik kijk er naar uit om eraan te werken</t>
+  </si>
+  <si>
+    <t>Verder gewerkt aan marketplaceusers flow</t>
+  </si>
+  <si>
+    <t>Vandaag heb ik verder gewerkt aan het opzetten van de nieuwe pagina. Eerst heb ik een testpagina gemaakt om te controleren
+of de API-call werkte en of ik de juiste gegevens terugkreeg. Zodra dat gelukt was, heb ik de call correct geïntegreerd in de code,
+op dezelfde manier als bij de bestaande implementaties.
+Daarna ben ik begonnen met het bouwen van de nieuwe pagina. Hiervoor kon ik een aantal componenten hergebruiken van de contactpagina,
+maar ik heb ook enkele nieuwe componenten moeten aanmaken.</t>
+  </si>
+  <si>
+    <t>bug fixing en unittesten</t>
+  </si>
+  <si>
+    <t>De marketplace flow was bijna afgerond dus heeft Quentin de laatste beetjes gedaan op woensdag. Vandaag heb ik eerst een kleine bug gefixt. De bug was dat er geen tekst verscheen tijdens het hoveren van een icoontje,
+dat kwam omdat de marketplaceconfig undefined was. Na dieper te zoeken kwam ik uit dat in de authreducer
+(waar al de configurations zitten) er geen marketplaceconfig bestond maar wel marketplaceconfiguration.
+Ik heb dan de naam aangepast overal waar dat gebruikt werd en dat werkte dan weer goed.
+De rest van de dag heb ik dan verder gewerkt aan testen te schrijven</t>
+  </si>
+  <si>
+    <t>Unittesten</t>
+  </si>
+  <si>
+    <t>Vandaag heb ik verder gewerkt aan het testen van ProfileCard,
+dat ging in het begin stroef maar naarmate de dag ging het een stuk beter en heb ik die ook kunnen afwerken</t>
+  </si>
+  <si>
+    <t>Vandaag heb ik een ander component getest namelijk ImageUploadModal, deze ging een stuk beter doordat ik veel test kon overnemen van
+ProfileCard, ik moest enkel paar info aanpassen. Dit duurde ook heel de dag omdat ik op het einde een moeilijk component moest testen
+namelijk om te zien of een image correct werd geupload. Deze nam meer tijd in beslag omdat ik de api call dat we doen naar de backend
+met ons foto moest ik mocken om de juiste response van hem te krijgen</t>
+  </si>
+  <si>
+    <t>bug fixing en laatste stageopdracht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vandaag heb ik in de voormiddag twee bugs opgelost. Die fouten werden gemeld door twee gebruikers en dankzij Sentry konden we ze snel opsporen. In het begin was het even wennen om met Sentry te werken, omdat het een andere manier van informatie tonen is dan wat je normaal in een ticket krijgt. Maar na het een paar keer goed doorgelezen te hebben, begreep ik hoe ik de errors moest interpreteren en oplossen.
+In de namiddag heb ik onderzoek gedaan voor mijn laatste stageopdracht. Die bestaat erin om een HTML-editor te ontwikkelen waarin gebruikers een e-mail kunnen schrijven, met daarnaast een live preview die automatisch wordt bijgewerkt terwijl ze typen. Het is een vrij complexe opdracht, maar ik kijk ernaar uit om hier de komende vier dagen verder aan te werken!
+</t>
+  </si>
+  <si>
+    <t>Email-editor</t>
+  </si>
+  <si>
+    <t>Vandaag heb ik verder gewerkt aan de e-mail preview. In het begin was het even nadenken hoe ik hier het best aan kon beginnen,
+maar na wat onderzoek besloot ik om het via een iframe op te lossen. Ik ben dan meteen aan de slag gegaan en had nog vóór de middag een nette,
+goed werkende e-maileditor klaar. Links op het scherm staat de HTML-editor, en rechts zie je de live preview van de e-mail.
+Die preview wordt automatisch geüpdatet zodra je 0,5 seconden niets meer typt.
+De opdracht voor de namiddag lag in dezelfde lijn. Ik moest een nieuwe pagina aanmaken waar gebruikers al hun e-mailtemplates kunnen bekijken.
+Daarnaast moeten ze op die pagina ook nieuwe templates kunnen toevoegen, bestaande templates bewerken
+een preview bekijken (zowel op laptop- als mobiel formaat), en een testmail kunnen versturen naar zichzelf.
+Vandaag ben ik er alvast in geslaagd om de eerste versie van die pagina af te werken, waarop je een overzicht ziet van
+alle eerder gemaakte e-mailtemplates.</t>
+  </si>
+  <si>
+    <t>Email page voor templates plus flow beginnen maken</t>
+  </si>
+  <si>
+    <t>Vandaag heb ik verder gewerkt aan de e-mailpagina. Aangezien we nog geen data uit de backend ontvangen,
+heb ik een JSON-bestand aangemaakt met mock-ups van e-mailtemplates. Vervolgens heb ik een EmailCard-component ontwikkeld
+om deze templates op een overzichtelijke en visueel aantrekkelijke manier weer te geven op het scherm.
+Daarna heb ik onze projectbrede Toolbar geïntegreerd, zodat gebruikers kunnen filteren op naam en sorteren op aanmaakdatum of laatste wijziging. Tot slot heb ik ervoor gezorgd dat wanneer je op een e-mailtemplate klikt, je wordt doorgestuurd naar de e-maileditor,
+waar je de template verder kunt bewerken.</t>
   </si>
 </sst>
 </file>
@@ -910,7 +1094,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -973,6 +1157,30 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1305,130 +1513,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0C2DE36-3BC9-4A2A-A33D-8BDA13B5750A}">
   <dimension ref="A1:G166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I117" sqref="I117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="87.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="87.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="20"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="37"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="45"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="9"/>
       <c r="F3" s="10"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="34"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="23"/>
       <c r="F5" s="10"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="42"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="23"/>
       <c r="F7" s="10"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="42"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="23"/>
       <c r="F9" s="10"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="D10" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="42"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="24"/>
       <c r="F11" s="10"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="34"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="42"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="25"/>
       <c r="C13" s="11"/>
@@ -1437,14 +1645,14 @@
       <c r="F13" s="12"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="21"/>
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="17" t="s">
         <v>6</v>
@@ -1463,7 +1671,7 @@
       </c>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="15">
         <v>1</v>
@@ -1482,7 +1690,7 @@
       </c>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="13">
         <v>2</v>
@@ -1501,7 +1709,7 @@
       </c>
       <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="13">
         <v>3</v>
@@ -1520,7 +1728,7 @@
       </c>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="13">
         <v>4</v>
@@ -1539,7 +1747,7 @@
       </c>
       <c r="G19" s="7"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="13">
         <v>5</v>
@@ -1558,7 +1766,7 @@
       </c>
       <c r="G20" s="7"/>
     </row>
-    <row r="21" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="13">
         <v>6</v>
@@ -1577,7 +1785,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="13">
         <v>7</v>
@@ -1596,7 +1804,7 @@
       </c>
       <c r="G22" s="7"/>
     </row>
-    <row r="23" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="13">
         <v>8</v>
@@ -1615,7 +1823,7 @@
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="13">
         <v>9</v>
@@ -1634,7 +1842,7 @@
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="13">
         <v>10</v>
@@ -1653,7 +1861,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="13">
         <v>11</v>
@@ -1672,7 +1880,7 @@
       </c>
       <c r="G26" s="7"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="13">
         <v>12</v>
@@ -1691,7 +1899,7 @@
       </c>
       <c r="G27" s="7"/>
     </row>
-    <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="13">
         <v>13</v>
@@ -1710,7 +1918,7 @@
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="13">
         <v>14</v>
@@ -1729,7 +1937,7 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="13">
         <v>15</v>
@@ -1748,7 +1956,7 @@
       </c>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="13">
         <v>16</v>
@@ -1767,7 +1975,7 @@
       </c>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="13">
         <v>17</v>
@@ -1786,7 +1994,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="13">
         <v>18</v>
@@ -1805,7 +2013,7 @@
       </c>
       <c r="G33" s="7"/>
     </row>
-    <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="13">
         <v>19</v>
@@ -1824,7 +2032,7 @@
       </c>
       <c r="G34" s="7"/>
     </row>
-    <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="13">
         <v>20</v>
@@ -1843,7 +2051,7 @@
       </c>
       <c r="G35" s="7"/>
     </row>
-    <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="13">
         <v>21</v>
@@ -1862,7 +2070,7 @@
       </c>
       <c r="G36" s="7"/>
     </row>
-    <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="13">
         <v>20</v>
@@ -1881,7 +2089,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="13">
         <v>23</v>
@@ -1900,7 +2108,7 @@
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="13">
         <v>21</v>
@@ -1919,7 +2127,7 @@
       </c>
       <c r="G39" s="7"/>
     </row>
-    <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="13">
         <v>25</v>
@@ -1938,7 +2146,7 @@
       </c>
       <c r="G40" s="7"/>
     </row>
-    <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="13">
         <v>25</v>
@@ -1957,7 +2165,7 @@
       </c>
       <c r="G41" s="7"/>
     </row>
-    <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="13">
         <v>21</v>
@@ -1976,7 +2184,7 @@
       </c>
       <c r="G42" s="7"/>
     </row>
-    <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="13">
         <v>28</v>
@@ -1995,7 +2203,7 @@
       </c>
       <c r="G43" s="7"/>
     </row>
-    <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="13">
         <v>29</v>
@@ -2014,7 +2222,7 @@
       </c>
       <c r="G44" s="7"/>
     </row>
-    <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="13">
         <v>30</v>
@@ -2033,7 +2241,7 @@
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="13">
         <v>31</v>
@@ -2052,7 +2260,7 @@
       </c>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="13">
         <v>32</v>
@@ -2071,7 +2279,7 @@
       </c>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="13">
         <v>33</v>
@@ -2090,7 +2298,7 @@
       </c>
       <c r="G48" s="7"/>
     </row>
-    <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="13">
         <v>34</v>
@@ -2109,7 +2317,7 @@
       </c>
       <c r="G49" s="7"/>
     </row>
-    <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="13">
         <v>35</v>
@@ -2128,7 +2336,7 @@
       </c>
       <c r="G50" s="7"/>
     </row>
-    <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="13">
         <v>36</v>
@@ -2147,7 +2355,7 @@
       </c>
       <c r="G51" s="7"/>
     </row>
-    <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="13">
         <v>37</v>
@@ -2166,7 +2374,7 @@
       </c>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="13">
         <v>38</v>
@@ -2185,7 +2393,7 @@
       </c>
       <c r="G53" s="7"/>
     </row>
-    <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="13">
         <v>39</v>
@@ -2204,7 +2412,7 @@
       </c>
       <c r="G54" s="7"/>
     </row>
-    <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="13">
         <v>40</v>
@@ -2223,7 +2431,7 @@
       </c>
       <c r="G55" s="7"/>
     </row>
-    <row r="56" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="13">
         <v>41</v>
@@ -2242,7 +2450,7 @@
       </c>
       <c r="G56" s="7"/>
     </row>
-    <row r="57" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="13">
         <v>42</v>
@@ -2261,7 +2469,7 @@
       </c>
       <c r="G57" s="7"/>
     </row>
-    <row r="58" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="13">
         <v>43</v>
@@ -2280,7 +2488,7 @@
       </c>
       <c r="G58" s="7"/>
     </row>
-    <row r="59" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="13">
         <v>44</v>
@@ -2299,7 +2507,7 @@
       </c>
       <c r="G59" s="7"/>
     </row>
-    <row r="60" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="13">
         <v>45</v>
@@ -2318,7 +2526,7 @@
       </c>
       <c r="G60" s="7"/>
     </row>
-    <row r="61" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="13">
         <v>46</v>
@@ -2337,7 +2545,7 @@
       </c>
       <c r="G61" s="7"/>
     </row>
-    <row r="62" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="13">
         <v>47</v>
@@ -2356,7 +2564,7 @@
       </c>
       <c r="G62" s="7"/>
     </row>
-    <row r="63" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="13">
         <v>48</v>
@@ -2375,7 +2583,7 @@
       </c>
       <c r="G63" s="7"/>
     </row>
-    <row r="64" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="13">
         <v>49</v>
@@ -2394,7 +2602,7 @@
       </c>
       <c r="G64" s="7"/>
     </row>
-    <row r="65" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="13">
         <v>50</v>
@@ -2413,7 +2621,7 @@
       </c>
       <c r="G65" s="7"/>
     </row>
-    <row r="66" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="13">
         <v>51</v>
@@ -2432,7 +2640,7 @@
       </c>
       <c r="G66" s="7"/>
     </row>
-    <row r="67" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="13">
         <v>52</v>
@@ -2451,7 +2659,7 @@
       </c>
       <c r="G67" s="7"/>
     </row>
-    <row r="68" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="13">
         <v>53</v>
@@ -2470,7 +2678,7 @@
       </c>
       <c r="G68" s="7"/>
     </row>
-    <row r="69" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="13">
         <v>54</v>
@@ -2489,7 +2697,7 @@
       </c>
       <c r="G69" s="7"/>
     </row>
-    <row r="70" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="13">
         <v>55</v>
@@ -2508,7 +2716,7 @@
       </c>
       <c r="G70" s="7"/>
     </row>
-    <row r="71" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="13">
         <v>56</v>
@@ -2527,7 +2735,7 @@
       </c>
       <c r="G71" s="7"/>
     </row>
-    <row r="72" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="13">
         <v>57</v>
@@ -2546,7 +2754,7 @@
       </c>
       <c r="G72" s="7"/>
     </row>
-    <row r="73" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="13">
         <v>58</v>
@@ -2565,7 +2773,7 @@
       </c>
       <c r="G73" s="7"/>
     </row>
-    <row r="74" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="13">
         <v>59</v>
@@ -2584,7 +2792,7 @@
       </c>
       <c r="G74" s="7"/>
     </row>
-    <row r="75" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="13">
         <v>60</v>
@@ -2603,7 +2811,7 @@
       </c>
       <c r="G75" s="7"/>
     </row>
-    <row r="76" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B76" s="13">
         <v>61</v>
       </c>
@@ -2620,7 +2828,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B77" s="13">
         <v>62</v>
       </c>
@@ -2637,7 +2845,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B78" s="13">
         <v>63</v>
       </c>
@@ -2654,7 +2862,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B79" s="13">
         <v>64</v>
       </c>
@@ -2671,7 +2879,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B80" s="13">
         <v>65</v>
       </c>
@@ -2688,7 +2896,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="81" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B81" s="13">
         <v>66</v>
       </c>
@@ -2705,7 +2913,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="82" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B82" s="13">
         <v>67</v>
       </c>
@@ -2722,7 +2930,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="83" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B83" s="13">
         <v>68</v>
       </c>
@@ -2739,7 +2947,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84" s="13">
         <v>69</v>
       </c>
@@ -2756,7 +2964,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" s="13">
         <v>70</v>
       </c>
@@ -2773,7 +2981,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86" s="13">
         <v>71</v>
       </c>
@@ -2790,7 +2998,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" s="13">
         <v>72</v>
       </c>
@@ -2807,7 +3015,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88" s="13">
         <v>73</v>
       </c>
@@ -2817,12 +3025,14 @@
       <c r="D88" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="E88" s="14"/>
+      <c r="E88" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="F88" s="14" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89" s="13">
         <v>74</v>
       </c>
@@ -2832,12 +3042,14 @@
       <c r="D89" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="E89" s="14"/>
+      <c r="E89" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="F89" s="14" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="90" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B90" s="13">
         <v>75</v>
       </c>
@@ -2847,12 +3059,14 @@
       <c r="D90" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="E90" s="14"/>
+      <c r="E90" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="F90" s="28" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="91" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B91" s="13">
         <v>76</v>
       </c>
@@ -2862,12 +3076,14 @@
       <c r="D91" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="E91" s="14"/>
+      <c r="E91" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="F91" s="28" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="92" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B92" s="13">
         <v>77</v>
       </c>
@@ -2877,12 +3093,14 @@
       <c r="D92" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="E92" s="14"/>
+      <c r="E92" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="F92" s="28" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="93" spans="2:6" ht="144" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B93" s="13">
         <v>78</v>
       </c>
@@ -2892,12 +3110,14 @@
       <c r="D93" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="E93" s="14"/>
+      <c r="E93" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="F93" s="28" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="94" spans="2:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B94" s="13">
         <v>79</v>
       </c>
@@ -2907,12 +3127,14 @@
       <c r="D94" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E94" s="14"/>
+      <c r="E94" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="F94" s="28" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="95" spans="2:6" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B95" s="13">
         <v>80</v>
       </c>
@@ -2922,12 +3144,14 @@
       <c r="D95" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E95" s="14"/>
+      <c r="E95" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="F95" s="28" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="96" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B96" s="13">
         <v>81</v>
       </c>
@@ -2937,12 +3161,14 @@
       <c r="D96" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="E96" s="14"/>
+      <c r="E96" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="F96" s="28" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="97" spans="2:6" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:6" ht="105" x14ac:dyDescent="0.25">
       <c r="B97" s="13">
         <v>82</v>
       </c>
@@ -2952,12 +3178,14 @@
       <c r="D97" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E97" s="14"/>
+      <c r="E97" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="F97" s="28" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="98" spans="2:6" ht="144" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:6" ht="105" x14ac:dyDescent="0.25">
       <c r="B98" s="13">
         <v>83</v>
       </c>
@@ -2967,12 +3195,14 @@
       <c r="D98" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E98" s="14"/>
+      <c r="E98" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="F98" s="28" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="99" spans="2:6" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:6" ht="180" x14ac:dyDescent="0.25">
       <c r="B99" s="13">
         <v>84</v>
       </c>
@@ -2982,201 +3212,353 @@
       <c r="D99" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="E99" s="14"/>
+      <c r="E99" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="F99" s="28" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B100" s="13">
         <v>85</v>
       </c>
-      <c r="C100" s="14"/>
-      <c r="D100" s="14"/>
-      <c r="E100" s="14"/>
-      <c r="F100" s="14"/>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C100" s="29">
+        <v>45764</v>
+      </c>
+      <c r="D100" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E100" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F100" s="28" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101" s="13">
         <v>86</v>
       </c>
-      <c r="C101" s="14"/>
-      <c r="D101" s="14"/>
-      <c r="E101" s="14"/>
-      <c r="F101" s="14"/>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C101" s="29">
+        <v>45765</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="E101" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F101" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" ht="105" x14ac:dyDescent="0.25">
       <c r="B102" s="13">
         <v>87</v>
       </c>
-      <c r="C102" s="14"/>
-      <c r="D102" s="14"/>
-      <c r="E102" s="14"/>
-      <c r="F102" s="14"/>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C102" s="29">
+        <v>45768</v>
+      </c>
+      <c r="D102" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="E102" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F102" s="28" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B103" s="13">
         <v>88</v>
       </c>
-      <c r="C103" s="14"/>
-      <c r="D103" s="14"/>
-      <c r="E103" s="14"/>
-      <c r="F103" s="14"/>
-    </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B104" s="13">
+      <c r="C103" s="29">
+        <v>45769</v>
+      </c>
+      <c r="D103" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E103" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F103" s="28" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B104" s="37">
         <v>89</v>
       </c>
-      <c r="C104" s="14"/>
-      <c r="D104" s="14"/>
-      <c r="E104" s="14"/>
-      <c r="F104" s="14"/>
-    </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B105" s="13">
-        <v>90</v>
-      </c>
-      <c r="C105" s="14"/>
-      <c r="D105" s="14"/>
-      <c r="E105" s="14"/>
-      <c r="F105" s="14"/>
-    </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C104" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="D104" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="E104" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="F104" s="35" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="38"/>
+      <c r="C105" s="40"/>
+      <c r="D105" s="34"/>
+      <c r="E105" s="34"/>
+      <c r="F105" s="36"/>
+    </row>
+    <row r="106" spans="2:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B106" s="13">
         <v>91</v>
       </c>
-      <c r="C106" s="14"/>
-      <c r="D106" s="14"/>
-      <c r="E106" s="14"/>
-      <c r="F106" s="14"/>
-    </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C106" s="29">
+        <v>45775</v>
+      </c>
+      <c r="D106" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E106" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F106" s="28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" ht="150" x14ac:dyDescent="0.25">
       <c r="B107" s="13">
         <v>92</v>
       </c>
-      <c r="C107" s="14"/>
-      <c r="D107" s="14"/>
-      <c r="E107" s="14"/>
-      <c r="F107" s="14"/>
-    </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C107" s="29">
+        <v>45776</v>
+      </c>
+      <c r="D107" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="E107" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F107" s="28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" ht="105" x14ac:dyDescent="0.25">
       <c r="B108" s="13">
         <v>93</v>
       </c>
-      <c r="C108" s="14"/>
-      <c r="D108" s="14"/>
-      <c r="E108" s="14"/>
-      <c r="F108" s="14"/>
-    </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C108" s="29">
+        <v>45782</v>
+      </c>
+      <c r="D108" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E108" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F108" s="28" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" ht="105" x14ac:dyDescent="0.25">
       <c r="B109" s="13">
         <v>94</v>
       </c>
-      <c r="C109" s="14"/>
-      <c r="D109" s="14"/>
-      <c r="E109" s="14"/>
-      <c r="F109" s="14"/>
-    </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C109" s="29">
+        <v>45783</v>
+      </c>
+      <c r="D109" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="E109" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F109" s="28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" ht="150" x14ac:dyDescent="0.25">
       <c r="B110" s="13">
         <v>95</v>
       </c>
-      <c r="C110" s="14"/>
-      <c r="D110" s="14"/>
-      <c r="E110" s="14"/>
-      <c r="F110" s="14"/>
-    </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C110" s="29">
+        <v>45785</v>
+      </c>
+      <c r="D110" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="E110" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F110" s="28" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6" ht="195" x14ac:dyDescent="0.25">
       <c r="B111" s="13">
         <v>96</v>
       </c>
-      <c r="C111" s="14"/>
-      <c r="D111" s="14"/>
-      <c r="E111" s="14"/>
-      <c r="F111" s="14"/>
-    </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C111" s="29">
+        <v>45789</v>
+      </c>
+      <c r="D111" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E111" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F111" s="28" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" ht="120" x14ac:dyDescent="0.25">
       <c r="B112" s="13">
         <v>97</v>
       </c>
-      <c r="C112" s="14"/>
-      <c r="D112" s="14"/>
-      <c r="E112" s="14"/>
-      <c r="F112" s="14"/>
-    </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C112" s="29">
+        <v>45790</v>
+      </c>
+      <c r="D112" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="E112" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F112" s="28" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B113" s="13">
         <v>98</v>
       </c>
-      <c r="C113" s="14"/>
-      <c r="D113" s="14"/>
-      <c r="E113" s="14"/>
-      <c r="F113" s="14"/>
-    </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C113" s="29">
+        <v>45792</v>
+      </c>
+      <c r="D113" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="E113" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F113" s="28" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B114" s="13">
         <v>99</v>
       </c>
-      <c r="C114" s="14"/>
-      <c r="D114" s="14"/>
-      <c r="E114" s="14"/>
-      <c r="F114" s="14"/>
-    </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C114" s="29">
+        <v>45796</v>
+      </c>
+      <c r="D114" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="E114" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F114" s="28" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" ht="105" x14ac:dyDescent="0.25">
       <c r="B115" s="13">
         <v>100</v>
       </c>
-      <c r="C115" s="14"/>
-      <c r="D115" s="14"/>
-      <c r="E115" s="14"/>
-      <c r="F115" s="14"/>
-    </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C115" s="29">
+        <v>45797</v>
+      </c>
+      <c r="D115" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="E115" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F115" s="28" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6" ht="180" x14ac:dyDescent="0.25">
       <c r="B116" s="13">
         <v>101</v>
       </c>
-      <c r="C116" s="14"/>
-      <c r="D116" s="14"/>
-      <c r="E116" s="14"/>
-      <c r="F116" s="14"/>
-    </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C116" s="29">
+        <v>45799</v>
+      </c>
+      <c r="D116" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="E116" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F116" s="28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6" ht="240" x14ac:dyDescent="0.25">
       <c r="B117" s="13">
         <v>102</v>
       </c>
-      <c r="C117" s="14"/>
-      <c r="D117" s="14"/>
-      <c r="E117" s="14"/>
-      <c r="F117" s="14"/>
-    </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C117" s="29">
+        <v>45803</v>
+      </c>
+      <c r="D117" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="E117" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F117" s="28" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="118" spans="2:6" ht="150" x14ac:dyDescent="0.25">
       <c r="B118" s="13">
         <v>103</v>
       </c>
-      <c r="C118" s="14"/>
-      <c r="D118" s="14"/>
-      <c r="E118" s="14"/>
-      <c r="F118" s="14"/>
-    </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C118" s="29">
+        <v>45804</v>
+      </c>
+      <c r="D118" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="E118" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F118" s="28" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119" s="13">
         <v>104</v>
       </c>
-      <c r="C119" s="14"/>
+      <c r="C119" s="29">
+        <v>45810</v>
+      </c>
       <c r="D119" s="14"/>
-      <c r="E119" s="14"/>
+      <c r="E119" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="F119" s="14"/>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B120" s="13">
         <v>105</v>
       </c>
-      <c r="C120" s="14"/>
+      <c r="C120" s="29">
+        <v>45811</v>
+      </c>
       <c r="D120" s="14"/>
-      <c r="E120" s="14"/>
+      <c r="E120" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="F120" s="14"/>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B121" s="13">
         <v>106</v>
       </c>
@@ -3185,7 +3567,7 @@
       <c r="E121" s="14"/>
       <c r="F121" s="14"/>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B122" s="13">
         <v>107</v>
       </c>
@@ -3194,7 +3576,7 @@
       <c r="E122" s="14"/>
       <c r="F122" s="14"/>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B123" s="13">
         <v>108</v>
       </c>
@@ -3203,7 +3585,7 @@
       <c r="E123" s="14"/>
       <c r="F123" s="14"/>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B124" s="13">
         <v>109</v>
       </c>
@@ -3212,7 +3594,7 @@
       <c r="E124" s="14"/>
       <c r="F124" s="14"/>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B125" s="13">
         <v>110</v>
       </c>
@@ -3221,7 +3603,7 @@
       <c r="E125" s="14"/>
       <c r="F125" s="14"/>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B126" s="13">
         <v>111</v>
       </c>
@@ -3230,7 +3612,7 @@
       <c r="E126" s="14"/>
       <c r="F126" s="14"/>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B127" s="13">
         <v>112</v>
       </c>
@@ -3239,7 +3621,7 @@
       <c r="E127" s="14"/>
       <c r="F127" s="14"/>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B128" s="13">
         <v>113</v>
       </c>
@@ -3248,7 +3630,7 @@
       <c r="E128" s="14"/>
       <c r="F128" s="14"/>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B129" s="13">
         <v>114</v>
       </c>
@@ -3257,7 +3639,7 @@
       <c r="E129" s="14"/>
       <c r="F129" s="14"/>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B130" s="13">
         <v>115</v>
       </c>
@@ -3266,7 +3648,7 @@
       <c r="E130" s="14"/>
       <c r="F130" s="14"/>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B131" s="13">
         <v>116</v>
       </c>
@@ -3275,7 +3657,7 @@
       <c r="E131" s="14"/>
       <c r="F131" s="14"/>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B132" s="13">
         <v>117</v>
       </c>
@@ -3284,7 +3666,7 @@
       <c r="E132" s="14"/>
       <c r="F132" s="14"/>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B133" s="13">
         <v>118</v>
       </c>
@@ -3293,7 +3675,7 @@
       <c r="E133" s="14"/>
       <c r="F133" s="14"/>
     </row>
-    <row r="134" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B134" s="13">
         <v>119</v>
       </c>
@@ -3302,7 +3684,7 @@
       <c r="E134" s="14"/>
       <c r="F134" s="14"/>
     </row>
-    <row r="135" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B135" s="13">
         <v>120</v>
       </c>
@@ -3311,7 +3693,7 @@
       <c r="E135" s="14"/>
       <c r="F135" s="14"/>
     </row>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B136" s="13">
         <v>121</v>
       </c>
@@ -3320,7 +3702,7 @@
       <c r="E136" s="14"/>
       <c r="F136" s="14"/>
     </row>
-    <row r="137" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B137" s="13">
         <v>122</v>
       </c>
@@ -3329,7 +3711,7 @@
       <c r="E137" s="14"/>
       <c r="F137" s="14"/>
     </row>
-    <row r="138" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B138" s="13">
         <v>123</v>
       </c>
@@ -3338,7 +3720,7 @@
       <c r="E138" s="14"/>
       <c r="F138" s="14"/>
     </row>
-    <row r="139" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B139" s="13">
         <v>124</v>
       </c>
@@ -3347,7 +3729,7 @@
       <c r="E139" s="14"/>
       <c r="F139" s="14"/>
     </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B140" s="13">
         <v>125</v>
       </c>
@@ -3356,7 +3738,7 @@
       <c r="E140" s="14"/>
       <c r="F140" s="14"/>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B141" s="13">
         <v>126</v>
       </c>
@@ -3365,7 +3747,7 @@
       <c r="E141" s="14"/>
       <c r="F141" s="14"/>
     </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B142" s="13">
         <v>127</v>
       </c>
@@ -3374,7 +3756,7 @@
       <c r="E142" s="14"/>
       <c r="F142" s="14"/>
     </row>
-    <row r="143" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B143" s="13">
         <v>128</v>
       </c>
@@ -3383,7 +3765,7 @@
       <c r="E143" s="14"/>
       <c r="F143" s="14"/>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B144" s="13">
         <v>129</v>
       </c>
@@ -3392,7 +3774,7 @@
       <c r="E144" s="14"/>
       <c r="F144" s="14"/>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B145" s="13">
         <v>130</v>
       </c>
@@ -3401,7 +3783,7 @@
       <c r="E145" s="14"/>
       <c r="F145" s="14"/>
     </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B146" s="13">
         <v>131</v>
       </c>
@@ -3410,7 +3792,7 @@
       <c r="E146" s="14"/>
       <c r="F146" s="14"/>
     </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B147" s="13">
         <v>132</v>
       </c>
@@ -3419,7 +3801,7 @@
       <c r="E147" s="14"/>
       <c r="F147" s="14"/>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B148" s="13">
         <v>133</v>
       </c>
@@ -3428,7 +3810,7 @@
       <c r="E148" s="14"/>
       <c r="F148" s="14"/>
     </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B149" s="13">
         <v>134</v>
       </c>
@@ -3437,7 +3819,7 @@
       <c r="E149" s="14"/>
       <c r="F149" s="14"/>
     </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B150" s="13">
         <v>135</v>
       </c>
@@ -3446,7 +3828,7 @@
       <c r="E150" s="14"/>
       <c r="F150" s="14"/>
     </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B151" s="13">
         <v>136</v>
       </c>
@@ -3455,7 +3837,7 @@
       <c r="E151" s="14"/>
       <c r="F151" s="14"/>
     </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B152" s="13">
         <v>137</v>
       </c>
@@ -3464,7 +3846,7 @@
       <c r="E152" s="14"/>
       <c r="F152" s="14"/>
     </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B153" s="13">
         <v>138</v>
       </c>
@@ -3473,7 +3855,7 @@
       <c r="E153" s="14"/>
       <c r="F153" s="14"/>
     </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B154" s="13">
         <v>139</v>
       </c>
@@ -3482,7 +3864,7 @@
       <c r="E154" s="14"/>
       <c r="F154" s="14"/>
     </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B155" s="13">
         <v>140</v>
       </c>
@@ -3491,7 +3873,7 @@
       <c r="E155" s="14"/>
       <c r="F155" s="14"/>
     </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B156" s="13">
         <v>141</v>
       </c>
@@ -3500,7 +3882,7 @@
       <c r="E156" s="14"/>
       <c r="F156" s="14"/>
     </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B157" s="13">
         <v>142</v>
       </c>
@@ -3509,7 +3891,7 @@
       <c r="E157" s="14"/>
       <c r="F157" s="14"/>
     </row>
-    <row r="158" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B158" s="13">
         <v>143</v>
       </c>
@@ -3518,7 +3900,7 @@
       <c r="E158" s="14"/>
       <c r="F158" s="14"/>
     </row>
-    <row r="159" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B159" s="13">
         <v>144</v>
       </c>
@@ -3527,7 +3909,7 @@
       <c r="E159" s="14"/>
       <c r="F159" s="14"/>
     </row>
-    <row r="160" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B160" s="13">
         <v>145</v>
       </c>
@@ -3536,7 +3918,7 @@
       <c r="E160" s="14"/>
       <c r="F160" s="14"/>
     </row>
-    <row r="161" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B161" s="13">
         <v>146</v>
       </c>
@@ -3545,7 +3927,7 @@
       <c r="E161" s="14"/>
       <c r="F161" s="14"/>
     </row>
-    <row r="162" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B162" s="13">
         <v>147</v>
       </c>
@@ -3554,7 +3936,7 @@
       <c r="E162" s="14"/>
       <c r="F162" s="14"/>
     </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B163" s="13">
         <v>148</v>
       </c>
@@ -3563,7 +3945,7 @@
       <c r="E163" s="14"/>
       <c r="F163" s="14"/>
     </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B164" s="13">
         <v>149</v>
       </c>
@@ -3572,7 +3954,7 @@
       <c r="E164" s="14"/>
       <c r="F164" s="14"/>
     </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B165" s="13">
         <v>150</v>
       </c>
@@ -3581,7 +3963,7 @@
       <c r="E165" s="14"/>
       <c r="F165" s="14"/>
     </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B166" s="13">
         <v>151</v>
       </c>
@@ -3591,13 +3973,18 @@
       <c r="F166" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="11">
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D104:D105"/>
+    <mergeCell ref="F104:F105"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="B104:B105"/>
+    <mergeCell ref="C104:C105"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
nieuws opvragen werkt, poster en rapport/werkstuk ook af
</commit_message>
<xml_diff>
--- a/stage/Logblad_Stage.xlsx
+++ b/stage/Logblad_Stage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbelm\Documenten\Graduaat-Programmeren\stage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCFD3C9-DA9F-4DEC-BF49-3223FD328D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BAD9D4-2266-4333-B288-680FB875E5A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{17B13AA9-2AFD-4646-A20A-7BB5FF3EC105}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="179">
   <si>
     <t>Logblad Stage</t>
   </si>
@@ -742,6 +742,22 @@
 om deze templates op een overzichtelijke en visueel aantrekkelijke manier weer te geven op het scherm.
 Daarna heb ik onze projectbrede Toolbar geïntegreerd, zodat gebruikers kunnen filteren op naam en sorteren op aanmaakdatum of laatste wijziging. Tot slot heb ik ervoor gezorgd dat wanneer je op een e-mailtemplate klikt, je wordt doorgestuurd naar de e-maileditor,
 waar je de template verder kunt bewerken.</t>
+  </si>
+  <si>
+    <t>EmailPage backend kopppelen met frontend</t>
+  </si>
+  <si>
+    <t>Vandaag was mijn laatste stagedag.
+Als afsluitende opdracht kreeg ik de taak om de previewpagina van de e-mails af te werken. Ik begon hier meteen aan en had deze vrij snel klaar. Daarna kreeg ik de kans om mijn volledige code nog eens grondig te testen en op verschillende plaatsen kleine verbeteringen door te voeren. Zo voegde ik bijvoorbeeld een veld toe om te tonen of een e-mailtemplate al gepubliceerd was of niet.
+Het was een zeer leerrijke stage, waarin ik veel verantwoordelijkheden kreeg en enorm veel heb bijgeleerd. Ik kijk met een positief gevoel terug op deze ervaring.</t>
+  </si>
+  <si>
+    <t>EmailPreview page aanmaken + laatste aanpassingen code</t>
+  </si>
+  <si>
+    <t>Vandaag werkte ik verder aan de e-mailpagina.
+ Vorige week heeft de backend developer de nodige API-calls voorzien voor het ophalen, aanmaken en updaten van e-mailtemplates. Vandaag heb ik deze integraties succesvol geïmplementeerd in mijn bestaande frontend-code en getest op correcte werking.
+Daarna ben ik gestart met mijn laatste opdracht: het opzetten van een nieuwe pagina waarop je een preview van de e-mails kunt bekijken in verschillende schermformaten, zoals desktop, laptop en mobiel. Dit is bedoeld om na te gaan hoe de e-mails zich gedragen op verschillende apparaten.</t>
   </si>
 </sst>
 </file>
@@ -1158,6 +1174,21 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1181,21 +1212,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1514,7 +1530,7 @@
   <dimension ref="A1:G166"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A116" zoomScale="82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I117" sqref="I117"/>
+      <selection activeCell="K118" sqref="K118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,13 +1553,13 @@
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="45"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1557,11 +1573,11 @@
       <c r="B4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="42"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="34"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1575,11 +1591,11 @@
       <c r="B6" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="41"/>
-      <c r="F6" s="42"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1593,11 +1609,11 @@
       <c r="B8" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="41"/>
-      <c r="F8" s="42"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1611,11 +1627,11 @@
       <c r="B10" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="42"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1629,11 +1645,11 @@
       <c r="B12" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="41"/>
-      <c r="F12" s="42"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="34"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -3288,28 +3304,28 @@
       </c>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B104" s="37">
+      <c r="B104" s="42">
         <v>89</v>
       </c>
-      <c r="C104" s="39" t="s">
+      <c r="C104" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="D104" s="33" t="s">
+      <c r="D104" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="E104" s="33" t="s">
+      <c r="E104" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="F104" s="35" t="s">
+      <c r="F104" s="40" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="105" spans="2:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="38"/>
-      <c r="C105" s="40"/>
-      <c r="D105" s="34"/>
-      <c r="E105" s="34"/>
-      <c r="F105" s="36"/>
+      <c r="B105" s="43"/>
+      <c r="C105" s="45"/>
+      <c r="D105" s="39"/>
+      <c r="E105" s="39"/>
+      <c r="F105" s="41"/>
     </row>
     <row r="106" spans="2:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B106" s="13">
@@ -3532,31 +3548,39 @@
         <v>174</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:6" ht="120" x14ac:dyDescent="0.25">
       <c r="B119" s="13">
         <v>104</v>
       </c>
       <c r="C119" s="29">
         <v>45810</v>
       </c>
-      <c r="D119" s="14"/>
+      <c r="D119" s="14" t="s">
+        <v>175</v>
+      </c>
       <c r="E119" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F119" s="14"/>
-    </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F119" s="28" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="120" spans="2:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B120" s="13">
         <v>105</v>
       </c>
       <c r="C120" s="29">
         <v>45811</v>
       </c>
-      <c r="D120" s="14"/>
+      <c r="D120" s="14" t="s">
+        <v>177</v>
+      </c>
       <c r="E120" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F120" s="14"/>
+      <c r="F120" s="28" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B121" s="13">
@@ -3974,17 +3998,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="D104:D105"/>
+    <mergeCell ref="F104:F105"/>
+    <mergeCell ref="E104:E105"/>
+    <mergeCell ref="B104:B105"/>
+    <mergeCell ref="C104:C105"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D104:D105"/>
-    <mergeCell ref="F104:F105"/>
-    <mergeCell ref="E104:E105"/>
-    <mergeCell ref="B104:B105"/>
-    <mergeCell ref="C104:C105"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3999,6 +4023,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E23CA4F9A7097943BB3661E90EAE6E4E" ma:contentTypeVersion="14" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="0d9e0f82b7cffe5fc1e74a09a28c1088">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9bca8325-008a-4bac-8c6f-d19d7077bb5c" xmlns:ns4="9ad299d5-20ee-4f22-8259-94c3717e0ced" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fa769e857125b647229b5c2d99e2d252" ns3:_="" ns4:_="">
     <xsd:import namespace="9bca8325-008a-4bac-8c6f-d19d7077bb5c"/>
@@ -4227,15 +4260,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{875E8F8E-7746-48C0-A297-237F1A7749C7}">
   <ds:schemaRefs>
@@ -4246,6 +4270,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8784147-5A1F-4134-92F8-D5D0439B0E8D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{259DE696-BD32-4CBC-931A-5C4B7B33C4BA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4262,12 +4294,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8784147-5A1F-4134-92F8-D5D0439B0E8D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>